<commit_message>
Fix in the PS table for first official menu for 2023
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2023_v1_0_0/PrescaleTable/L1Menu_Collisions2023_v1_0_0.xlsx
+++ b/official/L1Menu_Collisions2023_v1_0_0/PrescaleTable/L1Menu_Collisions2023_v1_0_0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2023_v1_0_0/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2023_v1_0_1/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2E97BB-DB28-8741-A47C-415B1FB03577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2E9FE8-251F-D047-AB9C-F2D411E75AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4560" yWindow="-17680" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="L1Menu_Collisions2023_v1_0_0" sheetId="1" r:id="rId1"/>
@@ -1359,7 +1359,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1387,13 +1387,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1430,14 +1425,8 @@
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1445,20 +1434,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFE0E0E0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1492,9 +1472,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1788,13 +1765,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD1013"/>
+  <dimension ref="A1:AD1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C359" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G367" sqref="G367"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6852,67 +6829,67 @@
         <v>0</v>
       </c>
       <c r="D69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -6926,67 +6903,67 @@
         <v>0</v>
       </c>
       <c r="D70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -7592,67 +7569,67 @@
         <v>0</v>
       </c>
       <c r="D79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -16703,7 +16680,7 @@
         <v>2</v>
       </c>
       <c r="G202" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H202" s="5">
         <v>1</v>
@@ -20690,7 +20667,7 @@
         <v>0</v>
       </c>
       <c r="D256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E256" s="5">
         <v>0</v>
@@ -20702,55 +20679,55 @@
         <v>0</v>
       </c>
       <c r="H256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X256" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -24538,7 +24515,7 @@
         <v>0</v>
       </c>
       <c r="D308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E308" s="5">
         <v>0</v>
@@ -24547,58 +24524,58 @@
         <v>0</v>
       </c>
       <c r="G308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X308" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29199,68 +29176,68 @@
       <c r="C371" s="5">
         <v>0</v>
       </c>
-      <c r="D371" s="13">
-        <v>250</v>
-      </c>
-      <c r="E371" s="13">
-        <v>250</v>
-      </c>
-      <c r="F371" s="13">
-        <v>250</v>
-      </c>
-      <c r="G371" s="13">
-        <v>250</v>
-      </c>
-      <c r="H371" s="13">
-        <v>250</v>
-      </c>
-      <c r="I371" s="13">
-        <v>250</v>
-      </c>
-      <c r="J371" s="13">
-        <v>250</v>
-      </c>
-      <c r="K371" s="13">
-        <v>250</v>
-      </c>
-      <c r="L371" s="13">
-        <v>250</v>
-      </c>
-      <c r="M371" s="13">
-        <v>250</v>
-      </c>
-      <c r="N371" s="13">
-        <v>250</v>
-      </c>
-      <c r="O371" s="13">
-        <v>250</v>
-      </c>
-      <c r="P371" s="13">
-        <v>250</v>
-      </c>
-      <c r="Q371" s="13">
-        <v>250</v>
-      </c>
-      <c r="R371" s="13">
-        <v>250</v>
-      </c>
-      <c r="S371" s="13">
-        <v>250</v>
-      </c>
-      <c r="T371" s="13">
-        <v>250</v>
-      </c>
-      <c r="U371" s="13">
-        <v>250</v>
-      </c>
-      <c r="V371" s="13">
-        <v>250</v>
-      </c>
-      <c r="W371" s="13">
-        <v>250</v>
-      </c>
-      <c r="X371" s="13">
-        <v>250</v>
+      <c r="D371" s="5">
+        <v>0</v>
+      </c>
+      <c r="E371" s="5">
+        <v>0</v>
+      </c>
+      <c r="F371" s="5">
+        <v>0</v>
+      </c>
+      <c r="G371" s="5">
+        <v>0</v>
+      </c>
+      <c r="H371" s="5">
+        <v>0</v>
+      </c>
+      <c r="I371" s="5">
+        <v>0</v>
+      </c>
+      <c r="J371" s="5">
+        <v>0</v>
+      </c>
+      <c r="K371" s="5">
+        <v>0</v>
+      </c>
+      <c r="L371" s="5">
+        <v>0</v>
+      </c>
+      <c r="M371" s="5">
+        <v>0</v>
+      </c>
+      <c r="N371" s="5">
+        <v>0</v>
+      </c>
+      <c r="O371" s="5">
+        <v>0</v>
+      </c>
+      <c r="P371" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q371" s="5">
+        <v>0</v>
+      </c>
+      <c r="R371" s="5">
+        <v>0</v>
+      </c>
+      <c r="S371" s="5">
+        <v>0</v>
+      </c>
+      <c r="T371" s="5">
+        <v>0</v>
+      </c>
+      <c r="U371" s="5">
+        <v>0</v>
+      </c>
+      <c r="V371" s="5">
+        <v>0</v>
+      </c>
+      <c r="W371" s="5">
+        <v>0</v>
+      </c>
+      <c r="X371" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="372" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29273,68 +29250,68 @@
       <c r="C372" s="5">
         <v>0</v>
       </c>
-      <c r="D372" s="13">
-        <v>1</v>
-      </c>
-      <c r="E372" s="13">
-        <v>1</v>
-      </c>
-      <c r="F372" s="13">
-        <v>1</v>
-      </c>
-      <c r="G372" s="13">
-        <v>1</v>
-      </c>
-      <c r="H372" s="13">
-        <v>1</v>
-      </c>
-      <c r="I372" s="13">
-        <v>1</v>
-      </c>
-      <c r="J372" s="13">
-        <v>1</v>
-      </c>
-      <c r="K372" s="13">
-        <v>1</v>
-      </c>
-      <c r="L372" s="13">
-        <v>1</v>
-      </c>
-      <c r="M372" s="13">
-        <v>1</v>
-      </c>
-      <c r="N372" s="13">
-        <v>1</v>
-      </c>
-      <c r="O372" s="13">
-        <v>1</v>
-      </c>
-      <c r="P372" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q372" s="13">
-        <v>1</v>
-      </c>
-      <c r="R372" s="13">
-        <v>1</v>
-      </c>
-      <c r="S372" s="13">
-        <v>1</v>
-      </c>
-      <c r="T372" s="13">
-        <v>1</v>
-      </c>
-      <c r="U372" s="13">
-        <v>1</v>
-      </c>
-      <c r="V372" s="13">
-        <v>1</v>
-      </c>
-      <c r="W372" s="13">
-        <v>1</v>
-      </c>
-      <c r="X372" s="13">
-        <v>1</v>
+      <c r="D372" s="5">
+        <v>0</v>
+      </c>
+      <c r="E372" s="5">
+        <v>0</v>
+      </c>
+      <c r="F372" s="5">
+        <v>0</v>
+      </c>
+      <c r="G372" s="5">
+        <v>0</v>
+      </c>
+      <c r="H372" s="5">
+        <v>0</v>
+      </c>
+      <c r="I372" s="5">
+        <v>0</v>
+      </c>
+      <c r="J372" s="5">
+        <v>0</v>
+      </c>
+      <c r="K372" s="5">
+        <v>0</v>
+      </c>
+      <c r="L372" s="5">
+        <v>0</v>
+      </c>
+      <c r="M372" s="5">
+        <v>0</v>
+      </c>
+      <c r="N372" s="5">
+        <v>0</v>
+      </c>
+      <c r="O372" s="5">
+        <v>0</v>
+      </c>
+      <c r="P372" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q372" s="5">
+        <v>0</v>
+      </c>
+      <c r="R372" s="5">
+        <v>0</v>
+      </c>
+      <c r="S372" s="5">
+        <v>0</v>
+      </c>
+      <c r="T372" s="5">
+        <v>0</v>
+      </c>
+      <c r="U372" s="5">
+        <v>0</v>
+      </c>
+      <c r="V372" s="5">
+        <v>0</v>
+      </c>
+      <c r="W372" s="5">
+        <v>0</v>
+      </c>
+      <c r="X372" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="373" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29347,68 +29324,68 @@
       <c r="C373" s="5">
         <v>0</v>
       </c>
-      <c r="D373" s="13">
-        <v>1</v>
-      </c>
-      <c r="E373" s="13">
-        <v>1</v>
-      </c>
-      <c r="F373" s="13">
-        <v>1</v>
-      </c>
-      <c r="G373" s="13">
-        <v>1</v>
-      </c>
-      <c r="H373" s="13">
-        <v>1</v>
-      </c>
-      <c r="I373" s="13">
-        <v>1</v>
-      </c>
-      <c r="J373" s="13">
-        <v>1</v>
-      </c>
-      <c r="K373" s="13">
-        <v>1</v>
-      </c>
-      <c r="L373" s="13">
-        <v>1</v>
-      </c>
-      <c r="M373" s="13">
-        <v>1</v>
-      </c>
-      <c r="N373" s="13">
-        <v>1</v>
-      </c>
-      <c r="O373" s="13">
-        <v>1</v>
-      </c>
-      <c r="P373" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q373" s="13">
-        <v>1</v>
-      </c>
-      <c r="R373" s="13">
-        <v>1</v>
-      </c>
-      <c r="S373" s="13">
-        <v>1</v>
-      </c>
-      <c r="T373" s="13">
-        <v>1</v>
-      </c>
-      <c r="U373" s="13">
-        <v>1</v>
-      </c>
-      <c r="V373" s="13">
-        <v>1</v>
-      </c>
-      <c r="W373" s="13">
-        <v>1</v>
-      </c>
-      <c r="X373" s="13">
-        <v>1</v>
+      <c r="D373" s="5">
+        <v>0</v>
+      </c>
+      <c r="E373" s="5">
+        <v>0</v>
+      </c>
+      <c r="F373" s="5">
+        <v>0</v>
+      </c>
+      <c r="G373" s="5">
+        <v>0</v>
+      </c>
+      <c r="H373" s="5">
+        <v>0</v>
+      </c>
+      <c r="I373" s="5">
+        <v>0</v>
+      </c>
+      <c r="J373" s="5">
+        <v>0</v>
+      </c>
+      <c r="K373" s="5">
+        <v>0</v>
+      </c>
+      <c r="L373" s="5">
+        <v>0</v>
+      </c>
+      <c r="M373" s="5">
+        <v>0</v>
+      </c>
+      <c r="N373" s="5">
+        <v>0</v>
+      </c>
+      <c r="O373" s="5">
+        <v>0</v>
+      </c>
+      <c r="P373" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q373" s="5">
+        <v>0</v>
+      </c>
+      <c r="R373" s="5">
+        <v>0</v>
+      </c>
+      <c r="S373" s="5">
+        <v>0</v>
+      </c>
+      <c r="T373" s="5">
+        <v>0</v>
+      </c>
+      <c r="U373" s="5">
+        <v>0</v>
+      </c>
+      <c r="V373" s="5">
+        <v>0</v>
+      </c>
+      <c r="W373" s="5">
+        <v>0</v>
+      </c>
+      <c r="X373" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="374" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29421,68 +29398,68 @@
       <c r="C374" s="5">
         <v>0</v>
       </c>
-      <c r="D374" s="13">
-        <v>100</v>
-      </c>
-      <c r="E374" s="13">
-        <v>100</v>
-      </c>
-      <c r="F374" s="13">
-        <v>100</v>
-      </c>
-      <c r="G374" s="13">
-        <v>100</v>
-      </c>
-      <c r="H374" s="13">
-        <v>100</v>
-      </c>
-      <c r="I374" s="13">
-        <v>100</v>
-      </c>
-      <c r="J374" s="13">
-        <v>100</v>
-      </c>
-      <c r="K374" s="13">
-        <v>100</v>
-      </c>
-      <c r="L374" s="13">
-        <v>100</v>
-      </c>
-      <c r="M374" s="13">
-        <v>100</v>
-      </c>
-      <c r="N374" s="13">
-        <v>100</v>
-      </c>
-      <c r="O374" s="13">
-        <v>100</v>
-      </c>
-      <c r="P374" s="13">
-        <v>100</v>
-      </c>
-      <c r="Q374" s="13">
-        <v>100</v>
-      </c>
-      <c r="R374" s="13">
-        <v>100</v>
-      </c>
-      <c r="S374" s="13">
-        <v>100</v>
-      </c>
-      <c r="T374" s="13">
-        <v>100</v>
-      </c>
-      <c r="U374" s="13">
-        <v>100</v>
-      </c>
-      <c r="V374" s="13">
-        <v>100</v>
-      </c>
-      <c r="W374" s="13">
-        <v>100</v>
-      </c>
-      <c r="X374" s="13">
-        <v>100</v>
+      <c r="D374" s="5">
+        <v>0</v>
+      </c>
+      <c r="E374" s="5">
+        <v>0</v>
+      </c>
+      <c r="F374" s="5">
+        <v>0</v>
+      </c>
+      <c r="G374" s="5">
+        <v>0</v>
+      </c>
+      <c r="H374" s="5">
+        <v>0</v>
+      </c>
+      <c r="I374" s="5">
+        <v>0</v>
+      </c>
+      <c r="J374" s="5">
+        <v>0</v>
+      </c>
+      <c r="K374" s="5">
+        <v>0</v>
+      </c>
+      <c r="L374" s="5">
+        <v>0</v>
+      </c>
+      <c r="M374" s="5">
+        <v>0</v>
+      </c>
+      <c r="N374" s="5">
+        <v>0</v>
+      </c>
+      <c r="O374" s="5">
+        <v>0</v>
+      </c>
+      <c r="P374" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q374" s="5">
+        <v>0</v>
+      </c>
+      <c r="R374" s="5">
+        <v>0</v>
+      </c>
+      <c r="S374" s="5">
+        <v>0</v>
+      </c>
+      <c r="T374" s="5">
+        <v>0</v>
+      </c>
+      <c r="U374" s="5">
+        <v>0</v>
+      </c>
+      <c r="V374" s="5">
+        <v>0</v>
+      </c>
+      <c r="W374" s="5">
+        <v>0</v>
+      </c>
+      <c r="X374" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="375" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29495,68 +29472,68 @@
       <c r="C375" s="5">
         <v>0</v>
       </c>
-      <c r="D375" s="13">
-        <v>20</v>
-      </c>
-      <c r="E375" s="13">
-        <v>20</v>
-      </c>
-      <c r="F375" s="13">
-        <v>20</v>
-      </c>
-      <c r="G375" s="13">
-        <v>20</v>
-      </c>
-      <c r="H375" s="13">
-        <v>20</v>
-      </c>
-      <c r="I375" s="13">
-        <v>20</v>
-      </c>
-      <c r="J375" s="13">
-        <v>20</v>
-      </c>
-      <c r="K375" s="13">
-        <v>20</v>
-      </c>
-      <c r="L375" s="13">
-        <v>20</v>
-      </c>
-      <c r="M375" s="13">
-        <v>20</v>
-      </c>
-      <c r="N375" s="13">
-        <v>20</v>
-      </c>
-      <c r="O375" s="13">
-        <v>20</v>
-      </c>
-      <c r="P375" s="13">
-        <v>20</v>
-      </c>
-      <c r="Q375" s="13">
-        <v>20</v>
-      </c>
-      <c r="R375" s="13">
-        <v>20</v>
-      </c>
-      <c r="S375" s="13">
-        <v>20</v>
-      </c>
-      <c r="T375" s="13">
-        <v>20</v>
-      </c>
-      <c r="U375" s="13">
-        <v>20</v>
-      </c>
-      <c r="V375" s="13">
-        <v>20</v>
-      </c>
-      <c r="W375" s="13">
-        <v>20</v>
-      </c>
-      <c r="X375" s="13">
-        <v>20</v>
+      <c r="D375" s="5">
+        <v>0</v>
+      </c>
+      <c r="E375" s="5">
+        <v>0</v>
+      </c>
+      <c r="F375" s="5">
+        <v>0</v>
+      </c>
+      <c r="G375" s="5">
+        <v>0</v>
+      </c>
+      <c r="H375" s="5">
+        <v>0</v>
+      </c>
+      <c r="I375" s="5">
+        <v>0</v>
+      </c>
+      <c r="J375" s="5">
+        <v>0</v>
+      </c>
+      <c r="K375" s="5">
+        <v>0</v>
+      </c>
+      <c r="L375" s="5">
+        <v>0</v>
+      </c>
+      <c r="M375" s="5">
+        <v>0</v>
+      </c>
+      <c r="N375" s="5">
+        <v>0</v>
+      </c>
+      <c r="O375" s="5">
+        <v>0</v>
+      </c>
+      <c r="P375" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q375" s="5">
+        <v>0</v>
+      </c>
+      <c r="R375" s="5">
+        <v>0</v>
+      </c>
+      <c r="S375" s="5">
+        <v>0</v>
+      </c>
+      <c r="T375" s="5">
+        <v>0</v>
+      </c>
+      <c r="U375" s="5">
+        <v>0</v>
+      </c>
+      <c r="V375" s="5">
+        <v>0</v>
+      </c>
+      <c r="W375" s="5">
+        <v>0</v>
+      </c>
+      <c r="X375" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="376" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29569,68 +29546,68 @@
       <c r="C376" s="5">
         <v>0</v>
       </c>
-      <c r="D376" s="13">
-        <v>1</v>
-      </c>
-      <c r="E376" s="13">
-        <v>1</v>
-      </c>
-      <c r="F376" s="13">
-        <v>1</v>
-      </c>
-      <c r="G376" s="13">
-        <v>1</v>
-      </c>
-      <c r="H376" s="13">
-        <v>1</v>
-      </c>
-      <c r="I376" s="13">
-        <v>1</v>
-      </c>
-      <c r="J376" s="13">
-        <v>1</v>
-      </c>
-      <c r="K376" s="13">
-        <v>1</v>
-      </c>
-      <c r="L376" s="13">
-        <v>1</v>
-      </c>
-      <c r="M376" s="13">
-        <v>1</v>
-      </c>
-      <c r="N376" s="13">
-        <v>1</v>
-      </c>
-      <c r="O376" s="13">
-        <v>1</v>
-      </c>
-      <c r="P376" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q376" s="13">
-        <v>1</v>
-      </c>
-      <c r="R376" s="13">
-        <v>1</v>
-      </c>
-      <c r="S376" s="13">
-        <v>1</v>
-      </c>
-      <c r="T376" s="13">
-        <v>1</v>
-      </c>
-      <c r="U376" s="13">
-        <v>1</v>
-      </c>
-      <c r="V376" s="13">
-        <v>1</v>
-      </c>
-      <c r="W376" s="13">
-        <v>1</v>
-      </c>
-      <c r="X376" s="13">
-        <v>1</v>
+      <c r="D376" s="5">
+        <v>0</v>
+      </c>
+      <c r="E376" s="5">
+        <v>0</v>
+      </c>
+      <c r="F376" s="5">
+        <v>0</v>
+      </c>
+      <c r="G376" s="5">
+        <v>0</v>
+      </c>
+      <c r="H376" s="5">
+        <v>0</v>
+      </c>
+      <c r="I376" s="5">
+        <v>0</v>
+      </c>
+      <c r="J376" s="5">
+        <v>0</v>
+      </c>
+      <c r="K376" s="5">
+        <v>0</v>
+      </c>
+      <c r="L376" s="5">
+        <v>0</v>
+      </c>
+      <c r="M376" s="5">
+        <v>0</v>
+      </c>
+      <c r="N376" s="5">
+        <v>0</v>
+      </c>
+      <c r="O376" s="5">
+        <v>0</v>
+      </c>
+      <c r="P376" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q376" s="5">
+        <v>0</v>
+      </c>
+      <c r="R376" s="5">
+        <v>0</v>
+      </c>
+      <c r="S376" s="5">
+        <v>0</v>
+      </c>
+      <c r="T376" s="5">
+        <v>0</v>
+      </c>
+      <c r="U376" s="5">
+        <v>0</v>
+      </c>
+      <c r="V376" s="5">
+        <v>0</v>
+      </c>
+      <c r="W376" s="5">
+        <v>0</v>
+      </c>
+      <c r="X376" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="377" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29643,68 +29620,68 @@
       <c r="C377" s="5">
         <v>0</v>
       </c>
-      <c r="D377" s="13">
-        <v>1</v>
-      </c>
-      <c r="E377" s="13">
-        <v>1</v>
-      </c>
-      <c r="F377" s="13">
-        <v>1</v>
-      </c>
-      <c r="G377" s="13">
-        <v>1</v>
-      </c>
-      <c r="H377" s="13">
-        <v>1</v>
-      </c>
-      <c r="I377" s="13">
-        <v>1</v>
-      </c>
-      <c r="J377" s="13">
-        <v>1</v>
-      </c>
-      <c r="K377" s="13">
-        <v>1</v>
-      </c>
-      <c r="L377" s="13">
-        <v>1</v>
-      </c>
-      <c r="M377" s="13">
-        <v>1</v>
-      </c>
-      <c r="N377" s="13">
-        <v>1</v>
-      </c>
-      <c r="O377" s="13">
-        <v>1</v>
-      </c>
-      <c r="P377" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q377" s="13">
-        <v>1</v>
-      </c>
-      <c r="R377" s="13">
-        <v>1</v>
-      </c>
-      <c r="S377" s="13">
-        <v>1</v>
-      </c>
-      <c r="T377" s="13">
-        <v>1</v>
-      </c>
-      <c r="U377" s="13">
-        <v>1</v>
-      </c>
-      <c r="V377" s="13">
-        <v>1</v>
-      </c>
-      <c r="W377" s="13">
-        <v>1</v>
-      </c>
-      <c r="X377" s="13">
-        <v>1</v>
+      <c r="D377" s="5">
+        <v>0</v>
+      </c>
+      <c r="E377" s="5">
+        <v>0</v>
+      </c>
+      <c r="F377" s="5">
+        <v>0</v>
+      </c>
+      <c r="G377" s="5">
+        <v>0</v>
+      </c>
+      <c r="H377" s="5">
+        <v>0</v>
+      </c>
+      <c r="I377" s="5">
+        <v>0</v>
+      </c>
+      <c r="J377" s="5">
+        <v>0</v>
+      </c>
+      <c r="K377" s="5">
+        <v>0</v>
+      </c>
+      <c r="L377" s="5">
+        <v>0</v>
+      </c>
+      <c r="M377" s="5">
+        <v>0</v>
+      </c>
+      <c r="N377" s="5">
+        <v>0</v>
+      </c>
+      <c r="O377" s="5">
+        <v>0</v>
+      </c>
+      <c r="P377" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q377" s="5">
+        <v>0</v>
+      </c>
+      <c r="R377" s="5">
+        <v>0</v>
+      </c>
+      <c r="S377" s="5">
+        <v>0</v>
+      </c>
+      <c r="T377" s="5">
+        <v>0</v>
+      </c>
+      <c r="U377" s="5">
+        <v>0</v>
+      </c>
+      <c r="V377" s="5">
+        <v>0</v>
+      </c>
+      <c r="W377" s="5">
+        <v>0</v>
+      </c>
+      <c r="X377" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="378" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29792,7 +29769,7 @@
         <v>17881</v>
       </c>
       <c r="D379" s="9">
-        <v>20219</v>
+        <v>18013</v>
       </c>
       <c r="E379" s="9">
         <v>18013</v>
@@ -29807,7 +29784,7 @@
         <v>18013</v>
       </c>
       <c r="I379" s="9">
-        <v>20219</v>
+        <v>18013</v>
       </c>
       <c r="J379" s="9">
         <v>18013</v>
@@ -29866,7 +29843,7 @@
         <v>0</v>
       </c>
       <c r="D380" s="9">
-        <v>13781</v>
+        <v>54039</v>
       </c>
       <c r="E380" s="9">
         <v>54039</v>
@@ -29881,7 +29858,7 @@
         <v>54039</v>
       </c>
       <c r="I380" s="9">
-        <v>13781</v>
+        <v>54039</v>
       </c>
       <c r="J380" s="9">
         <v>54039</v>
@@ -46899,109 +46876,26 @@
       <c r="W1010" s="5"/>
       <c r="X1010" s="5"/>
     </row>
-    <row r="1011" spans="3:24" ht="13" x14ac:dyDescent="0.15">
-      <c r="C1011" s="5"/>
-      <c r="D1011" s="5"/>
-      <c r="E1011" s="5"/>
-      <c r="F1011" s="5"/>
-      <c r="G1011" s="5"/>
-      <c r="H1011" s="5"/>
-      <c r="I1011" s="5"/>
-      <c r="J1011" s="5"/>
-      <c r="K1011" s="5"/>
-      <c r="L1011" s="5"/>
-      <c r="M1011" s="5"/>
-      <c r="N1011" s="5"/>
-      <c r="O1011" s="5"/>
-      <c r="P1011" s="5"/>
-      <c r="Q1011" s="5"/>
-      <c r="R1011" s="5"/>
-      <c r="S1011" s="5"/>
-      <c r="T1011" s="5"/>
-      <c r="U1011" s="5"/>
-      <c r="V1011" s="5"/>
-      <c r="W1011" s="5"/>
-      <c r="X1011" s="5"/>
-    </row>
-    <row r="1012" spans="3:24" ht="13" x14ac:dyDescent="0.15">
-      <c r="C1012" s="5"/>
-      <c r="D1012" s="5"/>
-      <c r="E1012" s="5"/>
-      <c r="F1012" s="5"/>
-      <c r="G1012" s="5"/>
-      <c r="H1012" s="5"/>
-      <c r="I1012" s="5"/>
-      <c r="J1012" s="5"/>
-      <c r="K1012" s="5"/>
-      <c r="L1012" s="5"/>
-      <c r="M1012" s="5"/>
-      <c r="N1012" s="5"/>
-      <c r="O1012" s="5"/>
-      <c r="P1012" s="5"/>
-      <c r="Q1012" s="5"/>
-      <c r="R1012" s="5"/>
-      <c r="S1012" s="5"/>
-      <c r="T1012" s="5"/>
-      <c r="U1012" s="5"/>
-      <c r="V1012" s="5"/>
-      <c r="W1012" s="5"/>
-      <c r="X1012" s="5"/>
-    </row>
-    <row r="1013" spans="3:24" ht="13" x14ac:dyDescent="0.15">
-      <c r="C1013" s="5"/>
-      <c r="D1013" s="5"/>
-      <c r="E1013" s="5"/>
-      <c r="F1013" s="5"/>
-      <c r="G1013" s="5"/>
-      <c r="H1013" s="5"/>
-      <c r="I1013" s="5"/>
-      <c r="J1013" s="5"/>
-      <c r="K1013" s="5"/>
-      <c r="L1013" s="5"/>
-      <c r="M1013" s="5"/>
-      <c r="N1013" s="5"/>
-      <c r="O1013" s="5"/>
-      <c r="P1013" s="5"/>
-      <c r="Q1013" s="5"/>
-      <c r="R1013" s="5"/>
-      <c r="S1013" s="5"/>
-      <c r="T1013" s="5"/>
-      <c r="U1013" s="5"/>
-      <c r="V1013" s="5"/>
-      <c r="W1013" s="5"/>
-      <c r="X1013" s="5"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C417">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+  <conditionalFormatting sqref="C2:C417 D248:W417">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:X246 D248:X370 D378:X417">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+  <conditionalFormatting sqref="X248:X417 D2:X246">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D371:X377">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix in PS table for first 2023 official menu
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2023_v1_0_0/PrescaleTable/L1Menu_Collisions2023_v1_0_0.xlsx
+++ b/official/L1Menu_Collisions2023_v1_0_0/PrescaleTable/L1Menu_Collisions2023_v1_0_0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2023_v1_0_1/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2023_v1_0_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2E9FE8-251F-D047-AB9C-F2D411E75AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C419BD-6A7F-6F47-8C7D-DCDD5DF1F287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4560" yWindow="-17680" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="L1Menu_Collisions2023_v1_0_0" sheetId="1" r:id="rId1"/>
@@ -1478,31 +1478,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE8B2"/>
-          <bgColor rgb="FFFCE8B2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4C7C3"/>
-          <bgColor rgb="FFF4C7C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1768,10 +1744,10 @@
   <dimension ref="A1:AD1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N347" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomRight" activeCell="R367" sqref="R367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29177,67 +29153,67 @@
         <v>0</v>
       </c>
       <c r="D371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="E371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="F371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="G371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="H371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="I371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="J371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="K371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="L371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="M371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="N371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="O371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="P371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="Q371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="R371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="S371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="T371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="U371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="V371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="W371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="X371" s="5">
-        <v>0</v>
+        <v>250</v>
       </c>
     </row>
     <row r="372" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29251,67 +29227,67 @@
         <v>0</v>
       </c>
       <c r="D372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X372" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="373" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29325,67 +29301,67 @@
         <v>0</v>
       </c>
       <c r="D373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X373" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="374" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29399,67 +29375,67 @@
         <v>0</v>
       </c>
       <c r="D374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="U374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="V374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="X374" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="375" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29473,67 +29449,67 @@
         <v>0</v>
       </c>
       <c r="D375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="P375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Q375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="S375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="X375" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="376" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29547,67 +29523,67 @@
         <v>0</v>
       </c>
       <c r="D376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X376" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="377" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -29621,67 +29597,67 @@
         <v>0</v>
       </c>
       <c r="D377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X377" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="378" spans="1:24" ht="13" x14ac:dyDescent="0.15">
@@ -46877,25 +46853,25 @@
       <c r="X1010" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C417 D248:W417">
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+  <conditionalFormatting sqref="C2:C417">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X248:X417 D2:X246">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+  <conditionalFormatting sqref="D2:X246 D248:X417">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>